<commit_message>
Add the REMIND-MAgPIE coupled model registration to the registration overview.
</commit_message>
<xml_diff>
--- a/ar6/model_registrations_overview.xlsx
+++ b/ar6/model_registrations_overview.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">IPCC AR6 Model Registrations</t>
   </si>
@@ -53,6 +53,21 @@
   </si>
   <si>
     <t xml:space="preserve">Uses EDGET model with transport specific energy service technologies and behavioral change. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.06.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMIND-MAgPIE 2.1-4.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPCC_AR6_model_registration_REMIND-MAgPIE_2.1-4.2.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Björn Sörgel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMIND – MAgPIE Coupled Version.</t>
   </si>
 </sst>
 </file>
@@ -67,6 +82,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -87,11 +103,13 @@
       <sz val="26"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -240,10 +258,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -252,7 +270,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="73.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="73.27"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -293,6 +311,23 @@
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added REMIND-MAgPIE 2.1-4.2 to overview spreadsheet
</commit_message>
<xml_diff>
--- a/ar6/model_registrations_overview.xlsx
+++ b/ar6/model_registrations_overview.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">IPCC AR6 Model Registrations</t>
   </si>
@@ -53,6 +53,21 @@
   </si>
   <si>
     <t xml:space="preserve">Uses EDGET model with transport specific energy service technologies and behavioral change. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.06.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMIND-MAgPIE 2.1-4.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPCC_AR6_model_registration_REMIND-MAgPIE_2.1-4.2.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bjoern Soergel, Alois Dirnaichner, Isabelle Weindl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupled system with latest REMIND and MAgPIE versions (e.g. for SDP)</t>
   </si>
 </sst>
 </file>
@@ -67,6 +82,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -87,11 +103,13 @@
       <sz val="26"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -240,19 +258,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="73.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="56.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="73.27"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -293,6 +311,23 @@
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added MAgPIE 4.2 stand-alone AR6 registration form
</commit_message>
<xml_diff>
--- a/ar6/model_registrations_overview.xlsx
+++ b/ar6/model_registrations_overview.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/OneDrive/Dokumente/PIK/Development/R/pik-piam/project_interfaces/ar6/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3EEFF6-E6A8-6B45-B11A-4DC369D2C539}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>IPCC AR6 Model Registrations</t>
   </si>
@@ -109,12 +115,27 @@
   </si>
   <si>
     <t>EDGE version used for EDGE paper 2019</t>
+  </si>
+  <si>
+    <t>08.07.2020</t>
+  </si>
+  <si>
+    <t>MAgPIE 4.2</t>
+  </si>
+  <si>
+    <t>IPCC_AR6_model_registration_MAgPIE_4.2.xlsx</t>
+  </si>
+  <si>
+    <t>Florian Humpenöder</t>
+  </si>
+  <si>
+    <t>MAgPIE 4.2 stand-alone version used for peatland paper</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -249,6 +270,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -296,7 +320,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -329,9 +353,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,6 +405,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -539,29 +597,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="54.28515625" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
-    <col min="5" max="5" width="73.28515625" style="1" customWidth="1"/>
-    <col min="6" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="11.5"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="54.33203125" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" customWidth="1"/>
+    <col min="5" max="5" width="73.33203125" style="1" customWidth="1"/>
+    <col min="6" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -578,7 +636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -595,7 +653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -612,7 +670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -629,7 +687,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -646,7 +704,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -663,7 +721,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -678,6 +736,23 @@
       </c>
       <c r="E10" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>